<commit_message>
added EV and EV/S/p
</commit_message>
<xml_diff>
--- a/6_notes.xlsx
+++ b/6_notes.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:II8"/>
+  <dimension ref="A1:II9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -7243,6 +7243,805 @@
         <v>33620456</v>
       </c>
     </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>ATGE</t>
+        </is>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>Education &amp; Training Services</t>
+        </is>
+      </c>
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>US</t>
+        </is>
+      </c>
+      <c r="D9" t="inlineStr">
+        <is>
+          <t>Adtalem Global Education Inc.</t>
+        </is>
+      </c>
+      <c r="E9" t="n">
+        <v>28.48</v>
+      </c>
+      <c r="F9" t="n">
+        <v>7</v>
+      </c>
+      <c r="G9" t="n">
+        <v>26.66</v>
+      </c>
+      <c r="H9" t="n">
+        <v>-35</v>
+      </c>
+      <c r="I9" t="n">
+        <v>43.85</v>
+      </c>
+      <c r="J9" t="n">
+        <v>50</v>
+      </c>
+      <c r="K9" t="n">
+        <v>87</v>
+      </c>
+      <c r="L9" t="n">
+        <v>0</v>
+      </c>
+      <c r="M9" t="n">
+        <v>1</v>
+      </c>
+      <c r="N9" t="n">
+        <v>24.24</v>
+      </c>
+      <c r="O9" t="n">
+        <v>94.51000000000001</v>
+      </c>
+      <c r="P9" t="n">
+        <v>-14.93</v>
+      </c>
+      <c r="Q9" t="n">
+        <v>5.74</v>
+      </c>
+      <c r="R9" t="n">
+        <v>7.44</v>
+      </c>
+      <c r="S9" t="n">
+        <v>78.47</v>
+      </c>
+      <c r="T9" t="n">
+        <v>0.89</v>
+      </c>
+      <c r="U9" t="n">
+        <v>-0.29</v>
+      </c>
+      <c r="V9" t="n">
+        <v>0</v>
+      </c>
+      <c r="W9" t="n">
+        <v>0.46</v>
+      </c>
+      <c r="X9" t="n">
+        <v>730464</v>
+      </c>
+      <c r="Y9" t="n">
+        <v>1417298688</v>
+      </c>
+      <c r="Z9" t="inlineStr">
+        <is>
+          <t>False</t>
+        </is>
+      </c>
+      <c r="AA9" t="n">
+        <v>12585</v>
+      </c>
+      <c r="AB9" t="inlineStr">
+        <is>
+          <t>2021-06-30</t>
+        </is>
+      </c>
+      <c r="AC9" t="inlineStr">
+        <is>
+          <t>USD</t>
+        </is>
+      </c>
+      <c r="AD9" t="inlineStr">
+        <is>
+          <t>2021-08-19</t>
+        </is>
+      </c>
+      <c r="AE9" t="inlineStr">
+        <is>
+          <t>2021-08-19</t>
+        </is>
+      </c>
+      <c r="AF9" t="n">
+        <v>2021</v>
+      </c>
+      <c r="AG9" t="inlineStr">
+        <is>
+          <t>FY</t>
+        </is>
+      </c>
+      <c r="AH9" t="n">
+        <v>1112380000</v>
+      </c>
+      <c r="AI9" t="n">
+        <v>489233000</v>
+      </c>
+      <c r="AJ9" t="n">
+        <v>623147000</v>
+      </c>
+      <c r="AK9" t="n">
+        <v>1</v>
+      </c>
+      <c r="AL9" t="n">
+        <v>0</v>
+      </c>
+      <c r="AM9" t="n">
+        <v>0</v>
+      </c>
+      <c r="AN9" t="n">
+        <v>0</v>
+      </c>
+      <c r="AO9" t="n">
+        <v>420267000</v>
+      </c>
+      <c r="AP9" t="n">
+        <v>0</v>
+      </c>
+      <c r="AQ9" t="n">
+        <v>420267000</v>
+      </c>
+      <c r="AR9" t="n">
+        <v>909500000</v>
+      </c>
+      <c r="AS9" t="n">
+        <v>4094000</v>
+      </c>
+      <c r="AT9" t="n">
+        <v>41365000</v>
+      </c>
+      <c r="AU9" t="n">
+        <v>99051000</v>
+      </c>
+      <c r="AV9" t="n">
+        <v>242573000</v>
+      </c>
+      <c r="AW9" t="n">
+        <v>0</v>
+      </c>
+      <c r="AX9" t="n">
+        <v>202880000</v>
+      </c>
+      <c r="AY9" t="n">
+        <v>0</v>
+      </c>
+      <c r="AZ9" t="n">
+        <v>76030000</v>
+      </c>
+      <c r="BA9" t="n">
+        <v>126850000</v>
+      </c>
+      <c r="BB9" t="n">
+        <v>0</v>
+      </c>
+      <c r="BC9" t="n">
+        <v>25248000</v>
+      </c>
+      <c r="BD9" t="n">
+        <v>76909000</v>
+      </c>
+      <c r="BE9" t="n">
+        <v>0</v>
+      </c>
+      <c r="BF9" t="n">
+        <v>2</v>
+      </c>
+      <c r="BG9" t="n">
+        <v>1</v>
+      </c>
+      <c r="BH9" t="n">
+        <v>51322000</v>
+      </c>
+      <c r="BI9" t="n">
+        <v>51645000</v>
+      </c>
+      <c r="BJ9" t="inlineStr">
+        <is>
+          <t>https://www.sec.gov/Archives/edgar/data/730464/000155837021011957/0001558370-21-011957-index.htm</t>
+        </is>
+      </c>
+      <c r="BK9" t="inlineStr">
+        <is>
+          <t>https://www.sec.gov/Archives/edgar/data/730464/000155837021011957/atge-20210630x10k.htm</t>
+        </is>
+      </c>
+      <c r="BL9" t="n">
+        <v>494613000</v>
+      </c>
+      <c r="BM9" t="n">
+        <v>0</v>
+      </c>
+      <c r="BN9" t="n">
+        <v>494613000</v>
+      </c>
+      <c r="BO9" t="n">
+        <v>67996000</v>
+      </c>
+      <c r="BP9" t="n">
+        <v>0</v>
+      </c>
+      <c r="BQ9" t="n">
+        <v>952344000</v>
+      </c>
+      <c r="BR9" t="n">
+        <v>1514953000</v>
+      </c>
+      <c r="BS9" t="n">
+        <v>466180000</v>
+      </c>
+      <c r="BT9" t="n">
+        <v>686374000</v>
+      </c>
+      <c r="BU9" t="n">
+        <v>276249000</v>
+      </c>
+      <c r="BV9" t="n">
+        <v>962623000</v>
+      </c>
+      <c r="BW9" t="n">
+        <v>0</v>
+      </c>
+      <c r="BX9" t="n">
+        <v>22479000</v>
+      </c>
+      <c r="BY9" t="n">
+        <v>87601000</v>
+      </c>
+      <c r="BZ9" t="n">
+        <v>1538883000</v>
+      </c>
+      <c r="CA9" t="n">
+        <v>0</v>
+      </c>
+      <c r="CB9" t="n">
+        <v>3053836000</v>
+      </c>
+      <c r="CC9" t="n">
+        <v>56071000</v>
+      </c>
+      <c r="CD9" t="n">
+        <v>58329000</v>
+      </c>
+      <c r="CE9" t="n">
+        <v>0</v>
+      </c>
+      <c r="CF9" t="n">
+        <v>100697000</v>
+      </c>
+      <c r="CG9" t="n">
+        <v>193710000</v>
+      </c>
+      <c r="CH9" t="n">
+        <v>408807000</v>
+      </c>
+      <c r="CI9" t="n">
+        <v>1235566000</v>
+      </c>
+      <c r="CJ9" t="n">
+        <v>0</v>
+      </c>
+      <c r="CK9" t="n">
+        <v>26991000</v>
+      </c>
+      <c r="CL9" t="n">
+        <v>81402000</v>
+      </c>
+      <c r="CM9" t="n">
+        <v>1343959000</v>
+      </c>
+      <c r="CN9" t="n">
+        <v>0</v>
+      </c>
+      <c r="CO9" t="n">
+        <v>223184000</v>
+      </c>
+      <c r="CP9" t="n">
+        <v>1752766000</v>
+      </c>
+      <c r="CQ9" t="n">
+        <v>0</v>
+      </c>
+      <c r="CR9" t="n">
+        <v>811000</v>
+      </c>
+      <c r="CS9" t="n">
+        <v>2005105000</v>
+      </c>
+      <c r="CT9" t="n">
+        <v>-7365000</v>
+      </c>
+      <c r="CU9" t="n">
+        <v>-697481000</v>
+      </c>
+      <c r="CV9" t="n">
+        <v>1301070000</v>
+      </c>
+      <c r="CW9" t="n">
+        <v>0</v>
+      </c>
+      <c r="CX9" t="n">
+        <v>1301070000</v>
+      </c>
+      <c r="CY9" t="n">
+        <v>3053836000</v>
+      </c>
+      <c r="CZ9" t="n">
+        <v>3053836000</v>
+      </c>
+      <c r="DA9" t="n">
+        <v>0</v>
+      </c>
+      <c r="DB9" t="n">
+        <v>1293895000</v>
+      </c>
+      <c r="DC9" t="n">
+        <v>799282000</v>
+      </c>
+      <c r="DD9" t="n">
+        <v>1519000</v>
+      </c>
+      <c r="DE9" t="n">
+        <v>13875000</v>
+      </c>
+      <c r="DF9" t="n">
+        <v>-7478000</v>
+      </c>
+      <c r="DG9" t="n">
+        <v>13259000</v>
+      </c>
+      <c r="DH9" t="n">
+        <v>8530000</v>
+      </c>
+      <c r="DI9" t="n">
+        <v>-6638000</v>
+      </c>
+      <c r="DJ9" t="n">
+        <v>8757000</v>
+      </c>
+      <c r="DK9" t="n">
+        <v>192199000</v>
+      </c>
+      <c r="DL9" t="n">
+        <v>0</v>
+      </c>
+      <c r="DM9" t="n">
+        <v>0</v>
+      </c>
+      <c r="DN9" t="n">
+        <v>-10745000</v>
+      </c>
+      <c r="DO9" t="n">
+        <v>2721000</v>
+      </c>
+      <c r="DP9" t="n">
+        <v>-48664000</v>
+      </c>
+      <c r="DQ9" t="n">
+        <v>-56688000</v>
+      </c>
+      <c r="DR9" t="n">
+        <v>-3000000</v>
+      </c>
+      <c r="DS9" t="n">
+        <v>0</v>
+      </c>
+      <c r="DT9" t="n">
+        <v>-100000000</v>
+      </c>
+      <c r="DU9" t="n">
+        <v>0</v>
+      </c>
+      <c r="DV9" t="n">
+        <v>779466000</v>
+      </c>
+      <c r="DW9" t="n">
+        <v>676466000</v>
+      </c>
+      <c r="DX9" t="n">
+        <v>534000</v>
+      </c>
+      <c r="DY9" t="n">
+        <v>812511000</v>
+      </c>
+      <c r="DZ9" t="n">
+        <v>1313616000</v>
+      </c>
+      <c r="EA9" t="n">
+        <v>501105000</v>
+      </c>
+      <c r="EB9" t="n">
+        <v>192199000</v>
+      </c>
+      <c r="EC9" t="n">
+        <v>-48664000</v>
+      </c>
+      <c r="ED9" t="n">
+        <v>143535000</v>
+      </c>
+      <c r="EE9" t="n">
+        <v>1289015800</v>
+      </c>
+      <c r="EF9" t="n">
+        <v>642125000</v>
+      </c>
+      <c r="EG9" t="n">
+        <v>433876000</v>
+      </c>
+      <c r="EH9" t="inlineStr">
+        <is>
+          <t>Adtalem Global Education Inc.</t>
+        </is>
+      </c>
+      <c r="EI9" t="n">
+        <v>-0</v>
+      </c>
+      <c r="EJ9" t="n">
+        <v>-0</v>
+      </c>
+      <c r="EK9" t="n">
+        <v>28</v>
+      </c>
+      <c r="EL9" t="n">
+        <v>29</v>
+      </c>
+      <c r="EM9" t="n">
+        <v>30</v>
+      </c>
+      <c r="EN9" t="n">
+        <v>35</v>
+      </c>
+      <c r="EO9" t="n">
+        <v>274479</v>
+      </c>
+      <c r="EP9" t="n">
+        <v>399448</v>
+      </c>
+      <c r="EQ9" t="inlineStr">
+        <is>
+          <t>NYSE</t>
+        </is>
+      </c>
+      <c r="ER9" t="n">
+        <v>29</v>
+      </c>
+      <c r="ES9" t="n">
+        <v>29</v>
+      </c>
+      <c r="ET9" t="n">
+        <v>0</v>
+      </c>
+      <c r="EU9" t="n">
+        <v>49764701</v>
+      </c>
+      <c r="EV9" t="n">
+        <v>1643525203</v>
+      </c>
+      <c r="EW9" t="n">
+        <v>1052001000</v>
+      </c>
+      <c r="EX9" t="n">
+        <v>395838000</v>
+      </c>
+      <c r="EY9" t="n">
+        <v>692766000</v>
+      </c>
+      <c r="EZ9" t="n">
+        <v>91589000</v>
+      </c>
+      <c r="FA9" t="n">
+        <v>345983000</v>
+      </c>
+      <c r="FB9" t="n">
+        <v>1310421000</v>
+      </c>
+      <c r="FC9" t="n">
+        <v>16275000</v>
+      </c>
+      <c r="FD9" t="n">
+        <v>107692000</v>
+      </c>
+      <c r="FE9" t="n">
+        <v>1239687000</v>
+      </c>
+      <c r="FF9" t="n">
+        <v>400411000</v>
+      </c>
+      <c r="FG9" t="n">
+        <v>504700000</v>
+      </c>
+      <c r="FH9" t="n">
+        <v>99790000</v>
+      </c>
+      <c r="FI9" t="n">
+        <v>311631000</v>
+      </c>
+      <c r="FJ9" t="n">
+        <v>1391530000</v>
+      </c>
+      <c r="FK9" t="n">
+        <v>348327000</v>
+      </c>
+      <c r="FL9" t="n">
+        <v>159479000</v>
+      </c>
+      <c r="FM9" t="n">
+        <v>709257000</v>
+      </c>
+      <c r="FN9" t="n">
+        <v>266654000</v>
+      </c>
+      <c r="FO9" t="n">
+        <v>635695000</v>
+      </c>
+      <c r="FP9" t="n">
+        <v>1265181000</v>
+      </c>
+      <c r="FQ9" t="n">
+        <v>1828317000</v>
+      </c>
+      <c r="FR9" t="n">
+        <v>1468222000</v>
+      </c>
+      <c r="FS9" t="n">
+        <v>40864000</v>
+      </c>
+      <c r="FT9" t="n">
+        <v>280374000</v>
+      </c>
+      <c r="FU9" t="n">
+        <v>107868000</v>
+      </c>
+      <c r="FV9" t="n">
+        <v>1514953000</v>
+      </c>
+      <c r="FW9" t="n">
+        <v>100697000</v>
+      </c>
+      <c r="FX9" t="n">
+        <v>408807000</v>
+      </c>
+      <c r="FY9" t="n">
+        <v>1301070000</v>
+      </c>
+      <c r="FZ9" t="n">
+        <v>1293895000</v>
+      </c>
+      <c r="GA9" t="n">
+        <v>799282000</v>
+      </c>
+      <c r="GB9" t="n">
+        <v>48036000</v>
+      </c>
+      <c r="GC9" t="n">
+        <v>280654000</v>
+      </c>
+      <c r="GD9" t="n">
+        <v>108500000</v>
+      </c>
+      <c r="GE9" t="n">
+        <v>1497278000</v>
+      </c>
+      <c r="GF9" t="n">
+        <v>116670000</v>
+      </c>
+      <c r="GG9" t="n">
+        <v>382205000</v>
+      </c>
+      <c r="GH9" t="n">
+        <v>1306224000</v>
+      </c>
+      <c r="GI9" t="n">
+        <v>792115000</v>
+      </c>
+      <c r="GJ9" t="n">
+        <v>80770000</v>
+      </c>
+      <c r="GK9" t="n">
+        <v>1192466000</v>
+      </c>
+      <c r="GL9" t="n">
+        <v>153136000</v>
+      </c>
+      <c r="GM9" t="n">
+        <v>-41545000</v>
+      </c>
+      <c r="GN9" t="n">
+        <v>31</v>
+      </c>
+      <c r="GO9" t="n">
+        <v>1</v>
+      </c>
+      <c r="GP9" t="n">
+        <v>399032</v>
+      </c>
+      <c r="GQ9" t="n">
+        <v>1526532096</v>
+      </c>
+      <c r="GR9" t="n">
+        <v>0</v>
+      </c>
+      <c r="GS9" t="inlineStr">
+        <is>
+          <t>26.66-43.85</t>
+        </is>
+      </c>
+      <c r="GT9" t="n">
+        <v>0</v>
+      </c>
+      <c r="GU9" t="inlineStr">
+        <is>
+          <t>USD</t>
+        </is>
+      </c>
+      <c r="GV9" t="inlineStr">
+        <is>
+          <t>US00737L1035</t>
+        </is>
+      </c>
+      <c r="GW9" t="inlineStr">
+        <is>
+          <t>00737L103</t>
+        </is>
+      </c>
+      <c r="GX9" t="inlineStr">
+        <is>
+          <t>NYSE</t>
+        </is>
+      </c>
+      <c r="GY9" t="inlineStr">
+        <is>
+          <t>https://www.adtalem.com</t>
+        </is>
+      </c>
+      <c r="GZ9" t="inlineStr">
+        <is>
+          <t>Adtalem Global Education Inc. provides workforce solutions worldwide. It operates through two segments, Medical and Healthcare; and Financial Services. The Medical and Healthcare segment offers degree and non-degree programs in the medical and healthcare postsecondary education industry. This segment operates Chamberlain University, American University of the Caribbean School of Medicine, Ross University School of Medicine, and Ross University School of Veterinary Medicine. The Financial Services segment provides test preparation, certifications, conferences, seminars, memberships, and subscriptions to business professionals in the areas of accounting, anti-money laundering, banking, and mortgage lending. It operates Association of Certified Anti-Money Laundering Specialists, Becker Professional Education, OnCourse Learning, and EduPristine. The company was formerly known as DeVry Education Group Inc. and changed its name to Adtalem Global Education Inc. in May 2017. Adtalem Global Education Inc. was incorporated in 1987 and is based in Chicago, Illinois.</t>
+        </is>
+      </c>
+      <c r="HA9" t="inlineStr">
+        <is>
+          <t>Ms. Lisa Wardell</t>
+        </is>
+      </c>
+      <c r="HB9" t="inlineStr">
+        <is>
+          <t>Consumer Defensive</t>
+        </is>
+      </c>
+      <c r="HC9" t="n">
+        <v>4426</v>
+      </c>
+      <c r="HD9" t="inlineStr">
+        <is>
+          <t>16305157700</t>
+        </is>
+      </c>
+      <c r="HE9" t="inlineStr">
+        <is>
+          <t>500 W Monroe St Fl 28</t>
+        </is>
+      </c>
+      <c r="HF9" t="inlineStr">
+        <is>
+          <t>Chicago</t>
+        </is>
+      </c>
+      <c r="HG9" t="inlineStr">
+        <is>
+          <t>ILLINOIS</t>
+        </is>
+      </c>
+      <c r="HH9" t="inlineStr">
+        <is>
+          <t>60661</t>
+        </is>
+      </c>
+      <c r="HI9" t="n">
+        <v>0</v>
+      </c>
+      <c r="HJ9" t="n">
+        <v>40</v>
+      </c>
+      <c r="HK9" t="inlineStr">
+        <is>
+          <t>https://fmpcloud.io/image-stock/ATGE.png</t>
+        </is>
+      </c>
+      <c r="HL9" t="inlineStr">
+        <is>
+          <t>1995-11-14</t>
+        </is>
+      </c>
+      <c r="HM9" t="inlineStr">
+        <is>
+          <t>False</t>
+        </is>
+      </c>
+      <c r="HN9" t="inlineStr">
+        <is>
+          <t>False</t>
+        </is>
+      </c>
+      <c r="HO9" t="inlineStr">
+        <is>
+          <t>True</t>
+        </is>
+      </c>
+      <c r="HP9" t="inlineStr">
+        <is>
+          <t>False</t>
+        </is>
+      </c>
+      <c r="HQ9" t="n">
+        <v>9108000</v>
+      </c>
+      <c r="HR9" t="n">
+        <v>-8201000</v>
+      </c>
+      <c r="HS9" t="n">
+        <v>1121488000</v>
+      </c>
+      <c r="HT9" t="n">
+        <v>1043800000</v>
+      </c>
+      <c r="HU9" t="n">
+        <v>165957000</v>
+      </c>
+      <c r="HV9" t="n">
+        <v>-15973000</v>
+      </c>
+      <c r="HW9" t="n">
+        <v>514284000</v>
+      </c>
+      <c r="HX9" t="n">
+        <v>264401000</v>
+      </c>
+      <c r="HY9" t="n">
+        <v>80086000</v>
+      </c>
+      <c r="HZ9" t="n">
+        <v>0</v>
+      </c>
+      <c r="IA9" t="n">
+        <v>26956530</v>
+      </c>
+      <c r="IB9" t="n">
+        <v>-68501530</v>
+      </c>
+      <c r="IC9" t="n">
+        <v>25</v>
+      </c>
+      <c r="ID9" t="n">
+        <v>84634470</v>
+      </c>
+      <c r="IE9" t="n">
+        <v>2</v>
+      </c>
+      <c r="IF9" t="n">
+        <v>73562000</v>
+      </c>
+      <c r="IG9" t="n">
+        <v>1</v>
+      </c>
+      <c r="IH9" t="n">
+        <v>0.05</v>
+      </c>
+      <c r="II9" t="n">
+        <v>-411018312</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>